<commit_message>
update to include tokenization process
</commit_message>
<xml_diff>
--- a/columns and entities.xlsx
+++ b/columns and entities.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1669e1487f32561/Tabs/Tabs/sentiment analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1669e1487f32561/Tabs/Tabs/sentiment analysis/supplementals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{8152EBE2-701C-4248-B28D-CCE887D0DBDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5A29DFCB-339C-49A2-B191-95DD5B383080}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{8152EBE2-701C-4248-B28D-CCE887D0DBDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DC19F84A-7CE3-489C-9499-9C3A79A632EA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{EBBB5AC7-440E-469F-91CD-1C8FC06F045E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="75">
   <si>
     <t>table_schema</t>
   </si>
@@ -184,7 +184,82 @@
     <t>SP_InsertInto_SentimentAnalysis</t>
   </si>
   <si>
-    <t>insert registry into sentiment analysis table</t>
+    <t>TBL_VOID_UserSessionInput</t>
+  </si>
+  <si>
+    <t>various inputs users put into Abyss</t>
+  </si>
+  <si>
+    <t>TBL_Tokens</t>
+  </si>
+  <si>
+    <t>tokens extracted from tokenization process</t>
+  </si>
+  <si>
+    <t>TBL_Tokens_Iteration</t>
+  </si>
+  <si>
+    <t>configuration parameters for tokenization process</t>
+  </si>
+  <si>
+    <t>VW_Tokens</t>
+  </si>
+  <si>
+    <t>recombining tokenization results with other metadata (date, input text, etc)</t>
+  </si>
+  <si>
+    <t>delete relevant staging tables in tokenization process</t>
+  </si>
+  <si>
+    <t>insert registry into tokenization iteration table</t>
+  </si>
+  <si>
+    <t>insert values into sentiment analysis table from staging table</t>
+  </si>
+  <si>
+    <t>insert values into tokenization table from staging table</t>
+  </si>
+  <si>
+    <t>PK_ID_Token</t>
+  </si>
+  <si>
+    <t>TS_Token</t>
+  </si>
+  <si>
+    <t>FK_ID_Token_Iteration</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>PK_ID_Tokens_Iteration</t>
+  </si>
+  <si>
+    <t>TS_Tokens_Iteration</t>
+  </si>
+  <si>
+    <t>TS_UserSessionInput</t>
+  </si>
+  <si>
+    <t>ID_User</t>
+  </si>
+  <si>
+    <t>ID_Session</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>TBL_VOID_Session</t>
+  </si>
+  <si>
+    <t>TBL_VOID_User</t>
+  </si>
+  <si>
+    <t>PK_ID_User</t>
+  </si>
+  <si>
+    <t>PK_ID_Session</t>
   </si>
 </sst>
 </file>
@@ -536,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3869663F-6ECD-42E5-9BC4-E9955C01B260}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,50 +632,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>48</v>
       </c>
-      <c r="B7" t="s">
-        <v>49</v>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -610,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37924BD1-1491-4D29-8A7F-B25F9BDFF627}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,10 +798,10 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -699,10 +830,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -731,10 +862,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -752,10 +883,10 @@
         <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -763,10 +894,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -784,10 +915,10 @@
         <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="J5" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -795,10 +926,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -807,7 +938,7 @@
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
         <v>32</v>
@@ -830,19 +961,19 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
@@ -856,13 +987,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -871,30 +1002,30 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
         <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I8" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -903,30 +1034,30 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -935,19 +1066,19 @@
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
         <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -955,22 +1086,22 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H11" t="s">
         <v>32</v>
@@ -987,10 +1118,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -999,7 +1130,7 @@
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G12" t="s">
         <v>32</v>
@@ -1016,13 +1147,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -1031,30 +1162,30 @@
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G13" t="s">
         <v>32</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="J13" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -1063,7 +1194,7 @@
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G14" t="s">
         <v>32</v>
@@ -1080,13 +1211,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -1115,30 +1246,478 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
         <v>29</v>
       </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
         <v>18</v>
       </c>
-      <c r="G16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" t="s">
+        <v>49</v>
+      </c>
+      <c r="J25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" t="s">
+        <v>49</v>
+      </c>
+      <c r="J27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>